<commit_message>
Correct 5x5 RGB BOM errors and add PCB spec
Added PCB specs to 5x5 RGB
Corrected BOM errors on 5x5 RGB
</commit_message>
<xml_diff>
--- a/RGB_IR Backlight 5x5/RGB-IR Backlight Separate RGB 5x5/Electrical/RGB_IR_J010131revC.xlsx
+++ b/RGB_IR Backlight 5x5/RGB-IR Backlight Separate RGB 5x5/Electrical/RGB_IR_J010131revC.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sawtelles\Documents\GitHub\LED-IR Backlight Separate RGB 5x5\Electrical\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sawtelles\Documents\GitHub\RGB-IR LED Boards\RGB_IR Backlight 5x5\RGB-IR Backlight Separate RGB 5x5\Electrical\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8838619-D163-428A-A544-A1437B581FAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E8DDD6B-27C9-4617-8688-AC1DB6E0BEE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-120" windowWidth="18240" windowHeight="28320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="J005794_RGB_IR" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">J005794_RGB_IR!$A$1:$I$40</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">J005794_RGB_IR!$A$1:$I$39</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="232">
   <si>
     <t>Qty</t>
   </si>
@@ -567,9 +567,6 @@
     <t>541-4.99CCT-ND</t>
   </si>
   <si>
-    <t>U24</t>
-  </si>
-  <si>
     <t>1 ch isolator</t>
   </si>
   <si>
@@ -591,24 +588,6 @@
     <t>445-7555-1-ND</t>
   </si>
   <si>
-    <t>IC REG LINEAR 3.3V 250MA SOT23-3</t>
-  </si>
-  <si>
-    <t>3.3V regulator</t>
-  </si>
-  <si>
-    <t>Diodes Incorporated</t>
-  </si>
-  <si>
-    <t>AP2138N-3.3TRG1</t>
-  </si>
-  <si>
-    <t>AP2138N-3.3TRG1DICT-ND</t>
-  </si>
-  <si>
-    <t>U25</t>
-  </si>
-  <si>
     <t>DC DC CONVERTER 5V 1W</t>
   </si>
   <si>
@@ -748,6 +727,9 @@
   </si>
   <si>
     <t xml:space="preserve">418-TRH160A2801213VI </t>
+  </si>
+  <si>
+    <t>U22</t>
   </si>
 </sst>
 </file>
@@ -1610,10 +1592,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:M55"/>
+  <dimension ref="A1:M54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D17" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M62" sqref="M62"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38:XFD38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1621,7 +1603,7 @@
     <col min="1" max="1" width="6.5703125" style="1" customWidth="1"/>
     <col min="2" max="2" width="19.42578125" style="4" customWidth="1"/>
     <col min="3" max="3" width="42.28515625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="30.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="44.5703125" style="1" customWidth="1"/>
     <col min="5" max="5" width="14.5703125" style="1" customWidth="1"/>
     <col min="6" max="6" width="23.85546875" style="1" customWidth="1"/>
     <col min="7" max="7" width="9.85546875" style="1" customWidth="1"/>
@@ -1635,7 +1617,7 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
@@ -1698,7 +1680,7 @@
         <v>30</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>28</v>
@@ -1716,7 +1698,7 @@
         <v>0.52</v>
       </c>
       <c r="J4" s="3">
-        <f t="shared" ref="J4:J39" si="0">A4*I4</f>
+        <f t="shared" ref="J4:J38" si="0">A4*I4</f>
         <v>1.56</v>
       </c>
       <c r="L4" s="5">
@@ -1739,7 +1721,7 @@
         <v>83</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="F5" s="1">
         <v>533984003</v>
@@ -1748,7 +1730,7 @@
         <v>57</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="I5" s="3">
         <v>0.85</v>
@@ -1758,7 +1740,7 @@
         <v>0.85</v>
       </c>
       <c r="L5" s="5">
-        <f t="shared" ref="L5:L39" si="1">A5*10</f>
+        <f t="shared" ref="L5:L38" si="1">A5*10</f>
         <v>10</v>
       </c>
       <c r="M5" s="3">
@@ -1847,7 +1829,7 @@
         <v>84</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>86</v>
@@ -1885,22 +1867,22 @@
         <v>1</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>85</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>57</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="I9" s="3">
         <v>28.5</v>
@@ -1929,7 +1911,7 @@
         <v>64</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>66</v>
@@ -1970,7 +1952,7 @@
         <v>111</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>55</v>
@@ -2011,7 +1993,7 @@
         <v>68</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>70</v>
@@ -2051,8 +2033,8 @@
       <c r="C13" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="D13" t="s">
-        <v>211</v>
+      <c r="D13" s="1" t="s">
+        <v>204</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>55</v>
@@ -2093,7 +2075,7 @@
         <v>91</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>212</v>
+        <v>205</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>55</v>
@@ -2133,8 +2115,8 @@
       <c r="C15" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="D15" t="s">
-        <v>213</v>
+      <c r="D15" s="1" t="s">
+        <v>206</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>55</v>
@@ -2164,7 +2146,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>24</v>
       </c>
@@ -2174,8 +2156,8 @@
       <c r="C16" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="D16" t="s">
-        <v>214</v>
+      <c r="D16" s="1" t="s">
+        <v>207</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>55</v>
@@ -2212,8 +2194,8 @@
       <c r="C17" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="D17" t="s">
-        <v>231</v>
+      <c r="D17" s="1" t="s">
+        <v>224</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>74</v>
@@ -2253,8 +2235,8 @@
       <c r="C18" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D18" t="s">
-        <v>215</v>
+      <c r="D18" s="1" t="s">
+        <v>208</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>55</v>
@@ -2335,8 +2317,8 @@
       <c r="C20" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="D20" t="s">
-        <v>216</v>
+      <c r="D20" s="1" t="s">
+        <v>209</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>51</v>
@@ -2376,8 +2358,8 @@
       <c r="C21" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D21" t="s">
-        <v>217</v>
+      <c r="D21" s="1" t="s">
+        <v>210</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>45</v>
@@ -2417,8 +2399,8 @@
       <c r="C22" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D22" t="s">
-        <v>218</v>
+      <c r="D22" s="1" t="s">
+        <v>211</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>35</v>
@@ -2459,7 +2441,7 @@
         <v>21</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>37</v>
@@ -2541,7 +2523,7 @@
         <v>79</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>45</v>
@@ -2623,7 +2605,7 @@
         <v>108</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="E27" s="2" t="s">
         <v>45</v>
@@ -2663,8 +2645,8 @@
       <c r="C28" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="D28" t="s">
-        <v>221</v>
+      <c r="D28" s="1" t="s">
+        <v>214</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>142</v>
@@ -2705,7 +2687,7 @@
         <v>147</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>149</v>
@@ -2746,10 +2728,10 @@
         <v>153</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="F30" s="1">
         <v>533984004</v>
@@ -2758,7 +2740,7 @@
         <v>57</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="I30" s="3">
         <v>1.02</v>
@@ -2827,8 +2809,8 @@
       <c r="C32" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="D32" t="s">
-        <v>223</v>
+      <c r="D32" s="1" t="s">
+        <v>216</v>
       </c>
       <c r="E32" s="1" t="s">
         <v>161</v>
@@ -2858,7 +2840,7 @@
         <v>723.19999999999993</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" ht="105" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>64</v>
       </c>
@@ -2868,8 +2850,8 @@
       <c r="C33" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="D33" t="s">
-        <v>225</v>
+      <c r="D33" s="1" t="s">
+        <v>218</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>161</v>
@@ -2899,7 +2881,7 @@
         <v>723.19999999999993</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" ht="105" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>64</v>
       </c>
@@ -2909,8 +2891,8 @@
       <c r="C34" s="4" t="s">
         <v>169</v>
       </c>
-      <c r="D34" t="s">
-        <v>224</v>
+      <c r="D34" s="1" t="s">
+        <v>217</v>
       </c>
       <c r="E34" s="1" t="s">
         <v>161</v>
@@ -2950,8 +2932,8 @@
       <c r="C35" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="D35" t="s">
-        <v>232</v>
+      <c r="D35" s="1" t="s">
+        <v>225</v>
       </c>
       <c r="E35" s="1" t="s">
         <v>174</v>
@@ -2986,25 +2968,25 @@
         <v>1</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>177</v>
+        <v>231</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="G36" s="1" t="s">
         <v>57</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
       <c r="I36" s="3">
         <v>4.4400000000000004</v>
@@ -3023,25 +3005,25 @@
         <v>4</v>
       </c>
       <c r="B37" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="C37" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="C37" s="4" t="s">
+      <c r="D37" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="E37" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="D37" t="s">
-        <v>230</v>
-      </c>
-      <c r="E37" s="1" t="s">
+      <c r="F37" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="F37" s="1" t="s">
+      <c r="G37" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="H37" s="1" t="s">
         <v>183</v>
-      </c>
-      <c r="G37" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="H37" s="1" t="s">
-        <v>184</v>
       </c>
       <c r="I37" s="3">
         <v>0.56999999999999995</v>
@@ -3055,18 +3037,18 @@
         <v>40</v>
       </c>
     </row>
-    <row r="38" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>1</v>
       </c>
       <c r="B38" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="D38" s="1" t="s">
         <v>186</v>
-      </c>
-      <c r="C38" s="4" t="s">
-        <v>185</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>190</v>
       </c>
       <c r="E38" s="1" t="s">
         <v>187</v>
@@ -3081,11 +3063,11 @@
         <v>189</v>
       </c>
       <c r="I38" s="3">
-        <v>0.38</v>
+        <v>18.38</v>
       </c>
       <c r="J38" s="3">
         <f t="shared" si="0"/>
-        <v>0.38</v>
+        <v>18.38</v>
       </c>
       <c r="L38" s="5">
         <f t="shared" si="1"/>
@@ -3093,199 +3075,162 @@
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A39" s="1">
-        <v>1</v>
-      </c>
-      <c r="B39" s="4" t="s">
-        <v>192</v>
-      </c>
-      <c r="C39" s="4" t="s">
-        <v>191</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="E39" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="F39" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="G39" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="H39" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="I39" s="3">
-        <v>18.38</v>
-      </c>
-      <c r="J39" s="3">
-        <f t="shared" si="0"/>
-        <v>18.38</v>
-      </c>
-      <c r="L39" s="5">
-        <f t="shared" si="1"/>
-        <v>10</v>
-      </c>
+      <c r="C39" s="4"/>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="C40" s="4"/>
-    </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="C40" s="4">
+        <f>0.25*8*B40/100</f>
+        <v>0.4</v>
+      </c>
+      <c r="J40" s="3" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B41" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="C41" s="4">
+        <f t="shared" ref="C41:C42" si="5">0.25*8*B41/100</f>
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B42" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="C41" s="4">
-        <f>0.25*8*B41/100</f>
+      <c r="C42" s="4">
+        <f t="shared" si="5"/>
         <v>0.4</v>
-      </c>
-      <c r="J41" s="3" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="42" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A42" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="B42" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="C42" s="4">
-        <f t="shared" ref="C42:C43" si="5">0.25*8*B42/100</f>
-        <v>0.6</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C43" s="4">
-        <f t="shared" si="5"/>
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A44" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="B44" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="C44" s="4">
-        <f xml:space="preserve"> 0.4 * 4 *B44/100</f>
+        <f xml:space="preserve"> 0.4 * 4 *B43/100</f>
         <v>0.8</v>
       </c>
     </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C45" s="4">
+        <f>SUM(C40:C43)</f>
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="C46" s="4">
-        <f>SUM(C41:C44)</f>
-        <v>2.2000000000000002</v>
-      </c>
-    </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="J47" s="3">
-        <f>SUM(J1:J40)</f>
-        <v>361.95399999999995</v>
-      </c>
-    </row>
-    <row r="48" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="B48" s="4" t="s">
+      <c r="J46" s="3">
+        <f>SUM(J1:J39)</f>
+        <v>361.57399999999996</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="B47" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="C48" s="1" t="s">
-        <v>233</v>
-      </c>
-      <c r="E48" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="F48" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="G48" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="H48" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="I48" s="3">
+      <c r="C47" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="H47" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="I47" s="3">
         <v>54</v>
       </c>
     </row>
-    <row r="52" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B51" s="4" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="52" spans="2:11" ht="60" x14ac:dyDescent="0.25">
       <c r="B52" s="4" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="53" spans="2:11" ht="60" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="G52" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="H52" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="I52" s="3">
+        <v>52.81</v>
+      </c>
+      <c r="K52" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="53" spans="2:11" ht="105" x14ac:dyDescent="0.25">
       <c r="B53" s="4" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="E53" s="1" t="s">
         <v>123</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>125</v>
+        <v>57</v>
       </c>
       <c r="H53" s="1" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="I53" s="3">
-        <v>52.81</v>
+        <v>61.64</v>
       </c>
       <c r="K53" s="1" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="54" spans="2:11" ht="105" x14ac:dyDescent="0.25">
-      <c r="B54" s="4" t="s">
-        <v>127</v>
-      </c>
+        <v>131</v>
+      </c>
+    </row>
+    <row r="54" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="E54" s="1" t="s">
-        <v>123</v>
+        <v>133</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="G54" s="1" t="s">
         <v>57</v>
       </c>
       <c r="H54" s="1" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="I54" s="3">
-        <v>61.64</v>
+        <v>57.93</v>
       </c>
       <c r="K54" s="1" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="55" spans="2:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="E55" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="F55" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="G55" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="H55" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="I55" s="3">
-        <v>57.93</v>
-      </c>
-      <c r="K55" s="1" t="s">
         <v>135</v>
       </c>
     </row>

</xml_diff>